<commit_message>
Primera excepción creada: Capital insuficiente.
</commit_message>
<xml_diff>
--- a/Resources/Stocks.xlsx
+++ b/Resources/Stocks.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G989"/>
+  <dimension ref="A1:G990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23182,7 +23182,7 @@
         <v>45173</v>
       </c>
       <c r="B989" t="n">
-        <v>634999.25</v>
+        <v>634999.1875</v>
       </c>
       <c r="C989" t="n">
         <v>641501.1875</v>
@@ -23197,6 +23197,29 @@
         <v>633243.3125</v>
       </c>
       <c r="G989" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="2" t="n">
+        <v>45174</v>
+      </c>
+      <c r="B990" t="n">
+        <v>633243.3125</v>
+      </c>
+      <c r="C990" t="n">
+        <v>633243.3125</v>
+      </c>
+      <c r="D990" t="n">
+        <v>597354.375</v>
+      </c>
+      <c r="E990" t="n">
+        <v>598133.375</v>
+      </c>
+      <c r="F990" t="n">
+        <v>598133.375</v>
+      </c>
+      <c r="G990" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>